<commit_message>
Test cases fixed and reading simulation sensor data file function added to agent
</commit_message>
<xml_diff>
--- a/NutrientSensorDataAfter.xlsx
+++ b/NutrientSensorDataAfter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratimasingh/Desktop/564-SoftwareDesign/greenhouse/src/main/java/services/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratimasingh/Desktop/564-SoftwareDesign/greenhouse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D88646-91B7-114F-B7B2-4DD06271D83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A12A57-0993-D946-B508-BC35C1E5CB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" xr2:uid="{762F17CD-487D-6840-BD50-5D408313316F}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>